<commit_message>
Escaleta guión 1 corregida
Se incluyeron ajustes de la coordinadora editorial
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion01/Escaleta_LE_06_01_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion01/Escaleta_LE_06_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Lenguaje\fuentes\contenidos\grado06\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csepulveda\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="320">
   <si>
     <t>Asignatura</t>
   </si>
@@ -661,18 +661,12 @@
     <t xml:space="preserve">Comprensión textual: el reportaje </t>
   </si>
   <si>
-    <t>Recurso M101AP-02</t>
-  </si>
-  <si>
     <t>La lectura de un reportaje</t>
   </si>
   <si>
     <t>Recurso M5D-01</t>
   </si>
   <si>
-    <t>Este recurso es completamente nuevo. Se debe orientar al estudiante para que redacte su propio reportaje</t>
-  </si>
-  <si>
     <t>Recurso M102AB-01</t>
   </si>
   <si>
@@ -712,15 +706,9 @@
     <t>Recurso elaborado por el autor. Aprobado para digitalizar pero incluir un ejemplo o información adicional para que el estudiante pueda resolver el ejercicio</t>
   </si>
   <si>
-    <t>Recurso elaborado por el autor.  Aprobado para digitalizar. El formato del recurso "M101" no aparece en la lista desplegable</t>
-  </si>
-  <si>
     <t>Recurso elaborado por el autor. Hay que reeditar el texto construido para hacerlo más sencillo y apuntar a explicar solamente el sustantivo y el adjetivo.</t>
   </si>
   <si>
-    <t>Recurso elaborado por el autor. Hay que reenfocar el recurso como inicialmente estaba planteado.</t>
-  </si>
-  <si>
     <t>En este recurso se busca que los estudiantes escuchen palabras y las clasifiquen en las categorías gramaticales vistas: sustantivo y adjetivo.</t>
   </si>
   <si>
@@ -730,9 +718,6 @@
     <t>Recurso elaborado por el autor. Sería muy buenbo hacer más extenso el texto a corregir, incluyendo más palabras con "k" y "q"</t>
   </si>
   <si>
-    <t>Recurso elaborado por el autor. Hay que replantear el recurso para enfocarlo a la escritura de un reportaje</t>
-  </si>
-  <si>
     <t>Practica: Lee y corrige el diálogo</t>
   </si>
   <si>
@@ -889,9 +874,6 @@
     <t>Actividad para comparar y clasificar elementos comunes en distintos textos informativos teniendo en cuenta sus principales características</t>
   </si>
   <si>
-    <t>Recurso elaborado por el autor. Aprobado para digitalizar pero hay que incluir más preguntas en él. Derecho Básico 8</t>
-  </si>
-  <si>
     <t>Derecho Básico 6</t>
   </si>
   <si>
@@ -901,9 +883,6 @@
     <t>Este es un recurso completamente nuevo. Se debe buscar un reportaje y plantear preguntas que permitan el desarrollo de la comprensión de lectura. Derecho Básico 3</t>
   </si>
   <si>
-    <t>Recurso elaborado por el autor. Hay que reeditar el recurso para que se enfoque más en el reportaje. Derecho Básico 10</t>
-  </si>
-  <si>
     <t>Recurso elaborado por el autor. Hay que replantear el recurso para que se den algunos pasos o requisitos para redactar reportajes en el formato F13B. Derecho Básico 2</t>
   </si>
   <si>
@@ -913,9 +892,6 @@
     <t>Los textos literarios y sus características</t>
   </si>
   <si>
-    <t>Este recurso corresponde al motor M101</t>
-  </si>
-  <si>
     <t>En este recurso el estudiante algunos rasgos que hacen que un texto sea literario</t>
   </si>
   <si>
@@ -986,6 +962,75 @@
   </si>
   <si>
     <t>Banco de actividades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurso elaborado por el autor.  Aprobado para digitalizar. El formato del recurso "M101" no aparece en la lista desplegable Debe convertirse en M101A. Así aparecerá en el GRECO:como un M101A. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurso elaborado por el autor. Aprobado para digitalizar pero hay que incluir más preguntas en él. Derecho Básico 8 Debe quedar como M101A </t>
+  </si>
+  <si>
+    <t>Este recurso corresponde al motor M101A</t>
+  </si>
+  <si>
+    <t>Recurso elaborado por el autor. Hay que reenfocar el recurso como inicialmente estaba planteado. Debe quedar como un M101A</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ecurso elaborado por el autor. Hay que reeditar el recurso para que se enfoque más en el reportaje. Debe ser un M101A. Derecho Básico 10</t>
+    </r>
+  </si>
+  <si>
+    <t>Recurso M101A-05</t>
+  </si>
+  <si>
+    <t>Ortografía: los grafemas q y k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: analiza casos del uso de llos grafemas q y k </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para afianzar la práctica de las reglas ortográficas de los grafemas q y k </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurso nuevo. Se pueden proponer párrafos donde se usen estas grafías y que los estudiantes expliquen su uso. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recursos M </t>
+  </si>
+  <si>
+    <t>Recurso M101A-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este recurso es completamente nuevo. Se debe orientar al estudiante para que redacte su propio reportaje. Cambié el motor. El título y la descripción es la misma. </t>
+  </si>
+  <si>
+    <t>Recurso M101A-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividades para repasar los contenidos del tema El reportaje </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se debe elaborar 10 preguntas abiertas. 3 de la sección de literatura. 2 de gramática, 2 de ortografía 2 de comprensión y 1 de producción. Sedebe marcar como gestor de actividades en la actividad didáctica. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se deben escribir actividades de todos los temas de esta unidad. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurso elaborado por el autor. Hay que replantear el recurso para enfocarlo a la escritura de un reportaje. Debe ser M101A y no M101AP. </t>
+  </si>
+  <si>
+    <t>Recurso M101A-08</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1459,12 +1504,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1486,6 +1525,55 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1766,127 +1854,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U116"/>
+  <dimension ref="A1:U117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T55" sqref="T55"/>
+    <sheetView tabSelected="1" topLeftCell="R43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.86328125" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="63.3984375" customWidth="1"/>
-    <col min="8" max="9" width="11.3984375" style="7"/>
-    <col min="10" max="10" width="101.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.73046875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.73046875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.42578125" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="7"/>
+    <col min="10" max="10" width="101.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="9" customWidth="1"/>
     <col min="13" max="13" width="14" style="9" customWidth="1"/>
-    <col min="14" max="14" width="15.1328125" customWidth="1"/>
-    <col min="15" max="15" width="92.59765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.1328125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.1328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="53.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="68.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="92.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="52" t="s">
+      <c r="N1" s="52"/>
+      <c r="O1" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="52" t="s">
+      <c r="T1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="50" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="56"/>
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="54"/>
       <c r="M2" s="17" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>68</v>
       </c>
@@ -1902,7 +1990,7 @@
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
       <c r="G3" s="35" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H3" s="36">
         <v>1</v>
@@ -1911,7 +1999,7 @@
         <v>125</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="K3" s="42" t="s">
         <v>69</v>
@@ -1924,7 +2012,7 @@
       </c>
       <c r="N3" s="48"/>
       <c r="O3" s="48" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="P3" s="46" t="s">
         <v>19</v>
@@ -1939,13 +2027,13 @@
         <v>127</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U3" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>68</v>
       </c>
@@ -1961,7 +2049,7 @@
       <c r="E4" s="29"/>
       <c r="F4" s="30"/>
       <c r="G4" s="35" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H4" s="36">
         <v>2</v>
@@ -1970,7 +2058,7 @@
         <v>125</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="K4" s="42" t="s">
         <v>69</v>
@@ -1983,7 +2071,7 @@
       </c>
       <c r="N4" s="48"/>
       <c r="O4" s="48" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="P4" s="46" t="s">
         <v>19</v>
@@ -1998,13 +2086,13 @@
         <v>127</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>68</v>
       </c>
@@ -2020,7 +2108,7 @@
       <c r="E5" s="29"/>
       <c r="F5" s="30"/>
       <c r="G5" s="35" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="H5" s="36">
         <v>3</v>
@@ -2029,7 +2117,7 @@
         <v>125</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="K5" s="42" t="s">
         <v>69</v>
@@ -2042,7 +2130,7 @@
       </c>
       <c r="N5" s="48"/>
       <c r="O5" s="48" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="P5" s="46" t="s">
         <v>19</v>
@@ -2063,7 +2151,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>68</v>
       </c>
@@ -2079,7 +2167,7 @@
       <c r="E6" s="29"/>
       <c r="F6" s="30"/>
       <c r="G6" s="35" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="H6" s="36">
         <v>4</v>
@@ -2088,7 +2176,7 @@
         <v>125</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="K6" s="42" t="s">
         <v>69</v>
@@ -2101,7 +2189,7 @@
       </c>
       <c r="N6" s="48"/>
       <c r="O6" s="48" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="P6" s="46" t="s">
         <v>19</v>
@@ -2116,13 +2204,13 @@
         <v>127</v>
       </c>
       <c r="T6" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="U6" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>68</v>
       </c>
@@ -2138,7 +2226,7 @@
       <c r="E7" s="29"/>
       <c r="F7" s="30"/>
       <c r="G7" s="35" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="H7" s="36">
         <v>5</v>
@@ -2147,7 +2235,7 @@
         <v>125</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="K7" s="42" t="s">
         <v>69</v>
@@ -2160,7 +2248,7 @@
       </c>
       <c r="N7" s="48"/>
       <c r="O7" s="48" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="P7" s="46" t="s">
         <v>19</v>
@@ -2175,72 +2263,72 @@
         <v>127</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="U7" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="27.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="35" t="s">
-        <v>295</v>
-      </c>
-      <c r="H8" s="36">
+      <c r="E8" s="69"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="84" t="s">
+        <v>287</v>
+      </c>
+      <c r="H8" s="71">
         <v>6</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="J8" s="37" t="s">
-        <v>292</v>
-      </c>
-      <c r="K8" s="42" t="s">
+      <c r="J8" s="73" t="s">
+        <v>284</v>
+      </c>
+      <c r="K8" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="43" t="s">
+      <c r="L8" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48" t="s">
-        <v>284</v>
-      </c>
-      <c r="P8" s="46" t="s">
+      <c r="M8" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75" t="s">
+        <v>303</v>
+      </c>
+      <c r="P8" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="85">
         <v>6</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="R8" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="S8" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="T8" s="14" t="s">
+      <c r="T8" s="83" t="s">
         <v>162</v>
       </c>
-      <c r="U8" s="4" t="s">
+      <c r="U8" s="82" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>68</v>
       </c>
@@ -2267,7 +2355,7 @@
         <v>120</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="K9" s="42" t="s">
         <v>70</v>
@@ -2278,7 +2366,7 @@
       <c r="M9" s="48"/>
       <c r="N9" s="48"/>
       <c r="O9" s="47" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P9" s="46" t="s">
         <v>19</v>
@@ -2299,68 +2387,68 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="38" t="s">
+      <c r="F10" s="70"/>
+      <c r="G10" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="71">
         <v>8</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="J10" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="K10" s="42" t="s">
+      <c r="J10" s="73" t="s">
+        <v>268</v>
+      </c>
+      <c r="K10" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="43" t="s">
+      <c r="L10" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="48" t="s">
-        <v>63</v>
+      <c r="M10" s="75" t="s">
+        <v>62</v>
       </c>
       <c r="N10" s="48"/>
-      <c r="O10" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="P10" s="46" t="s">
+      <c r="O10" s="60" t="s">
+        <v>302</v>
+      </c>
+      <c r="P10" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10" s="63">
         <v>6</v>
       </c>
-      <c r="R10" s="13" t="s">
+      <c r="R10" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="S10" s="13" t="s">
+      <c r="S10" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="T10" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="U10" s="4" t="s">
+      <c r="T10" s="82" t="s">
+        <v>179</v>
+      </c>
+      <c r="U10" s="82" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>68</v>
       </c>
@@ -2389,7 +2477,7 @@
         <v>125</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="K11" s="44" t="s">
         <v>69</v>
@@ -2402,7 +2490,7 @@
       </c>
       <c r="N11" s="48"/>
       <c r="O11" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P11" s="46" t="s">
         <v>19</v>
@@ -2423,7 +2511,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>68</v>
       </c>
@@ -2452,7 +2540,7 @@
         <v>120</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="K12" s="44" t="s">
         <v>69</v>
@@ -2465,7 +2553,7 @@
         <v>37</v>
       </c>
       <c r="O12" s="47" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="P12" s="46" t="s">
         <v>19</v>
@@ -2486,7 +2574,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>68</v>
       </c>
@@ -2526,7 +2614,7 @@
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
       <c r="O13" s="47" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="P13" s="46" t="s">
         <v>19</v>
@@ -2547,7 +2635,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>68</v>
       </c>
@@ -2606,7 +2694,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>68</v>
       </c>
@@ -2626,7 +2714,7 @@
         <v>97</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H15" s="36">
         <v>13</v>
@@ -2648,7 +2736,7 @@
       </c>
       <c r="N15" s="48"/>
       <c r="O15" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P15" s="46" t="s">
         <v>19</v>
@@ -2669,7 +2757,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>68</v>
       </c>
@@ -2728,7 +2816,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="27.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>68</v>
       </c>
@@ -2757,7 +2845,7 @@
         <v>140</v>
       </c>
       <c r="J17" s="37" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="K17" s="44" t="s">
         <v>69</v>
@@ -2770,7 +2858,7 @@
         <v>41</v>
       </c>
       <c r="O17" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P17" s="46" t="s">
         <v>19</v>
@@ -2791,7 +2879,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>68</v>
       </c>
@@ -2850,7 +2938,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>68</v>
       </c>
@@ -2879,7 +2967,7 @@
         <v>125</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="K19" s="44" t="s">
         <v>69</v>
@@ -2892,7 +2980,7 @@
       </c>
       <c r="N19" s="48"/>
       <c r="O19" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P19" s="46" t="s">
         <v>19</v>
@@ -2913,7 +3001,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>68</v>
       </c>
@@ -2942,7 +3030,7 @@
         <v>140</v>
       </c>
       <c r="J20" s="37" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="K20" s="44" t="s">
         <v>69</v>
@@ -2955,7 +3043,7 @@
         <v>41</v>
       </c>
       <c r="O20" s="47" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P20" s="46" t="s">
         <v>19</v>
@@ -2976,7 +3064,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>68</v>
       </c>
@@ -3005,7 +3093,7 @@
         <v>125</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="K21" s="44" t="s">
         <v>69</v>
@@ -3018,7 +3106,7 @@
       </c>
       <c r="N21" s="48"/>
       <c r="O21" s="47" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P21" s="46" t="s">
         <v>19</v>
@@ -3039,7 +3127,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>68</v>
       </c>
@@ -3068,7 +3156,7 @@
         <v>140</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="K22" s="44" t="s">
         <v>69</v>
@@ -3081,7 +3169,7 @@
         <v>41</v>
       </c>
       <c r="O22" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P22" s="46" t="s">
         <v>19</v>
@@ -3102,7 +3190,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="27.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>68</v>
       </c>
@@ -3120,7 +3208,7 @@
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="38" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H23" s="36">
         <v>21</v>
@@ -3140,7 +3228,7 @@
       <c r="M23" s="48"/>
       <c r="N23" s="48"/>
       <c r="O23" s="47" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="P23" s="46" t="s">
         <v>19</v>
@@ -3161,7 +3249,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>68</v>
       </c>
@@ -3179,7 +3267,7 @@
       </c>
       <c r="F24" s="30"/>
       <c r="G24" s="38" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H24" s="36">
         <v>22</v>
@@ -3218,8 +3306,8 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="22" t="s">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58" t="s">
         <v>68</v>
       </c>
       <c r="B25" s="23" t="s">
@@ -3236,7 +3324,7 @@
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="38" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H25" s="36">
         <v>23</v>
@@ -3245,7 +3333,7 @@
         <v>125</v>
       </c>
       <c r="J25" s="37" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="K25" s="44" t="s">
         <v>70</v>
@@ -3275,68 +3363,68 @@
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="22" t="s">
+    <row r="26" spans="1:21" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="H26" s="36">
+      <c r="F26" s="70"/>
+      <c r="G26" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="H26" s="71">
         <v>24</v>
       </c>
-      <c r="I26" s="39" t="s">
+      <c r="I26" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="J26" s="37" t="s">
-        <v>257</v>
-      </c>
-      <c r="K26" s="44" t="s">
+      <c r="J26" s="73" t="s">
+        <v>252</v>
+      </c>
+      <c r="K26" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L26" s="45" t="s">
+      <c r="L26" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="M26" s="51" t="s">
-        <v>63</v>
+      <c r="M26" s="59" t="s">
+        <v>62</v>
       </c>
       <c r="N26" s="48"/>
-      <c r="O26" s="47" t="s">
-        <v>217</v>
+      <c r="O26" s="60" t="s">
+        <v>301</v>
       </c>
       <c r="P26" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="Q26" s="1">
+      <c r="Q26" s="63">
         <v>6</v>
       </c>
-      <c r="R26" s="13" t="s">
+      <c r="R26" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="S26" s="13" t="s">
+      <c r="S26" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="T26" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="U26" s="2" t="s">
+      <c r="T26" s="64" t="s">
+        <v>193</v>
+      </c>
+      <c r="U26" s="65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>68</v>
       </c>
@@ -3347,7 +3435,7 @@
         <v>91</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>103</v>
@@ -3363,7 +3451,7 @@
         <v>140</v>
       </c>
       <c r="J27" s="37" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="K27" s="44" t="s">
         <v>69</v>
@@ -3376,7 +3464,7 @@
         <v>36</v>
       </c>
       <c r="O27" s="47" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="P27" s="46" t="s">
         <v>19</v>
@@ -3397,7 +3485,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>68</v>
       </c>
@@ -3456,7 +3544,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>68</v>
       </c>
@@ -3483,7 +3571,7 @@
         <v>125</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="K29" s="44" t="s">
         <v>70</v>
@@ -3515,68 +3603,68 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A30" s="22" t="s">
+    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="H30" s="36">
+      <c r="F30" s="88"/>
+      <c r="G30" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="H30" s="71">
         <v>28</v>
       </c>
-      <c r="I30" s="39" t="s">
+      <c r="I30" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="J30" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="K30" s="44" t="s">
+      <c r="J30" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="K30" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L30" s="45" t="s">
+      <c r="L30" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="M30" s="51" t="s">
-        <v>63</v>
+      <c r="M30" s="59" t="s">
+        <v>62</v>
       </c>
       <c r="N30" s="48"/>
-      <c r="O30" s="47" t="s">
-        <v>219</v>
-      </c>
-      <c r="P30" s="46" t="s">
+      <c r="O30" s="60" t="s">
+        <v>304</v>
+      </c>
+      <c r="P30" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q30" s="63">
         <v>6</v>
       </c>
-      <c r="R30" s="13" t="s">
+      <c r="R30" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="S30" s="13" t="s">
+      <c r="S30" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="T30" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="U30" s="2" t="s">
+      <c r="T30" s="64" t="s">
+        <v>299</v>
+      </c>
+      <c r="U30" s="65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>68</v>
       </c>
@@ -3594,7 +3682,7 @@
       </c>
       <c r="F31" s="32"/>
       <c r="G31" s="38" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H31" s="36">
         <v>29</v>
@@ -3603,7 +3691,7 @@
         <v>125</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="K31" s="44" t="s">
         <v>69</v>
@@ -3616,7 +3704,7 @@
       </c>
       <c r="N31" s="48"/>
       <c r="O31" s="47" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P31" s="46" t="s">
         <v>19</v>
@@ -3631,13 +3719,13 @@
         <v>127</v>
       </c>
       <c r="T31" s="13" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="U31" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>68</v>
       </c>
@@ -3650,10 +3738,12 @@
       <c r="D32" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E32" s="31"/>
+      <c r="E32" s="31" t="s">
+        <v>102</v>
+      </c>
       <c r="F32" s="32"/>
       <c r="G32" s="38" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H32" s="36">
         <v>30</v>
@@ -3662,7 +3752,7 @@
         <v>140</v>
       </c>
       <c r="J32" s="40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K32" s="44" t="s">
         <v>69</v>
@@ -3675,7 +3765,7 @@
         <v>36</v>
       </c>
       <c r="O32" s="47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="P32" s="46" t="s">
         <v>19</v>
@@ -3690,13 +3780,13 @@
         <v>133</v>
       </c>
       <c r="T32" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="U32" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>68</v>
       </c>
@@ -3723,7 +3813,7 @@
         <v>125</v>
       </c>
       <c r="J33" s="37" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="K33" s="44" t="s">
         <v>69</v>
@@ -3736,7 +3826,7 @@
       </c>
       <c r="N33" s="48"/>
       <c r="O33" s="47" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P33" s="46" t="s">
         <v>19</v>
@@ -3757,7 +3847,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>68</v>
       </c>
@@ -3784,7 +3874,7 @@
         <v>125</v>
       </c>
       <c r="J34" s="37" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="K34" s="44" t="s">
         <v>69</v>
@@ -3797,7 +3887,7 @@
       </c>
       <c r="N34" s="48"/>
       <c r="O34" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P34" s="46" t="s">
         <v>19</v>
@@ -3818,7 +3908,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>68</v>
       </c>
@@ -3858,7 +3948,7 @@
       </c>
       <c r="N35" s="48"/>
       <c r="O35" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P35" s="46" t="s">
         <v>19</v>
@@ -3879,7 +3969,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>68</v>
       </c>
@@ -3906,7 +3996,7 @@
         <v>125</v>
       </c>
       <c r="J36" s="37" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="K36" s="44" t="s">
         <v>69</v>
@@ -3919,7 +4009,7 @@
       </c>
       <c r="N36" s="48"/>
       <c r="O36" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P36" s="46"/>
       <c r="Q36" s="1">
@@ -3938,7 +4028,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>68</v>
       </c>
@@ -3956,7 +4046,7 @@
       </c>
       <c r="F37" s="32"/>
       <c r="G37" s="38" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H37" s="36">
         <v>35</v>
@@ -3978,7 +4068,7 @@
       </c>
       <c r="N37" s="48"/>
       <c r="O37" s="47" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P37" s="46" t="s">
         <v>19</v>
@@ -3993,74 +4083,72 @@
         <v>127</v>
       </c>
       <c r="T37" s="4" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="U37" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
-      <c r="A38" s="22" t="s">
+    <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="D38" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" s="31" t="s">
+      <c r="D38" s="86" t="s">
+        <v>307</v>
+      </c>
+      <c r="E38" s="87" t="s">
         <v>102</v>
       </c>
       <c r="F38" s="32"/>
-      <c r="G38" s="38" t="s">
-        <v>233</v>
-      </c>
-      <c r="H38" s="36">
-        <v>36</v>
-      </c>
-      <c r="I38" s="39" t="s">
+      <c r="G38" s="41" t="s">
+        <v>308</v>
+      </c>
+      <c r="H38" s="71"/>
+      <c r="I38" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="J38" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="K38" s="44" t="s">
+      <c r="J38" s="73" t="s">
+        <v>309</v>
+      </c>
+      <c r="K38" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L38" s="45" t="s">
+      <c r="L38" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="M38" s="48" t="s">
-        <v>58</v>
+      <c r="M38" s="75" t="s">
+        <v>24</v>
       </c>
       <c r="N38" s="48"/>
-      <c r="O38" s="47" t="s">
-        <v>222</v>
-      </c>
-      <c r="P38" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q38" s="1">
+      <c r="O38" s="60" t="s">
+        <v>310</v>
+      </c>
+      <c r="P38" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q38" s="63">
         <v>6</v>
       </c>
-      <c r="R38" s="13" t="s">
+      <c r="R38" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="S38" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="T38" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="U38" s="2" t="s">
+      <c r="S38" s="64" t="s">
+        <v>311</v>
+      </c>
+      <c r="T38" s="89" t="s">
+        <v>306</v>
+      </c>
+      <c r="U38" s="82" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="43" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>68</v>
       </c>
@@ -4071,57 +4159,57 @@
         <v>91</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>199</v>
+        <v>119</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F39" s="32"/>
       <c r="G39" s="38" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
       <c r="H39" s="36">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I39" s="39" t="s">
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="J39" s="37" t="s">
-        <v>266</v>
+        <v>197</v>
       </c>
       <c r="K39" s="44" t="s">
         <v>69</v>
       </c>
       <c r="L39" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="M39" s="48"/>
-      <c r="N39" s="48" t="s">
-        <v>35</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M39" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="N39" s="48"/>
       <c r="O39" s="47" t="s">
-        <v>278</v>
+        <v>218</v>
       </c>
       <c r="P39" s="46" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q39" s="1">
         <v>6</v>
       </c>
       <c r="R39" s="13" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="S39" s="13" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="T39" s="13" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>68</v>
       </c>
@@ -4135,33 +4223,33 @@
         <v>199</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F40" s="32"/>
       <c r="G40" s="38" t="s">
-        <v>201</v>
+        <v>262</v>
       </c>
       <c r="H40" s="36">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I40" s="39" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="J40" s="37" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="K40" s="44" t="s">
         <v>69</v>
       </c>
       <c r="L40" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="M40" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="N40" s="48"/>
+        <v>31</v>
+      </c>
+      <c r="M40" s="48"/>
+      <c r="N40" s="48" t="s">
+        <v>35</v>
+      </c>
       <c r="O40" s="47" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="P40" s="46" t="s">
         <v>19</v>
@@ -4170,19 +4258,19 @@
         <v>6</v>
       </c>
       <c r="R40" s="13" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="S40" s="13" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="T40" s="13" t="s">
-        <v>303</v>
+        <v>191</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>68</v>
       </c>
@@ -4196,26 +4284,54 @@
         <v>199</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F41" s="32"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="48"/>
+      <c r="G41" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="H41" s="36">
+        <v>38</v>
+      </c>
+      <c r="I41" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="J41" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="K41" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="M41" s="48" t="s">
+        <v>84</v>
+      </c>
       <c r="N41" s="48"/>
-      <c r="O41" s="47"/>
-      <c r="P41" s="46"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="13"/>
-      <c r="T41" s="13"/>
-      <c r="U41" s="2"/>
-    </row>
-    <row r="42" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
+      <c r="O41" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="P41" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>6</v>
+      </c>
+      <c r="R41" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="S41" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="T41" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="U41" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>68</v>
       </c>
@@ -4229,245 +4345,217 @@
         <v>199</v>
       </c>
       <c r="E42" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" s="32"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="45"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="48"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="46"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="2"/>
+    </row>
+    <row r="43" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="86" t="s">
+        <v>199</v>
+      </c>
+      <c r="E43" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="38" t="s">
-        <v>234</v>
-      </c>
-      <c r="H42" s="36">
+      <c r="F43" s="88"/>
+      <c r="G43" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="H43" s="71">
         <v>39</v>
       </c>
-      <c r="I42" s="39" t="s">
+      <c r="I43" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="J42" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="K42" s="44" t="s">
+      <c r="J43" s="73" t="s">
+        <v>270</v>
+      </c>
+      <c r="K43" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L42" s="45" t="s">
+      <c r="L43" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="M42" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="N42" s="48"/>
-      <c r="O42" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="P42" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q42" s="1">
-        <v>6</v>
-      </c>
-      <c r="R42" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="S42" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="T42" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="U42" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
-      <c r="A43" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="E43" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F43" s="32"/>
-      <c r="G43" s="38" t="s">
-        <v>251</v>
-      </c>
-      <c r="H43" s="36">
-        <v>40</v>
-      </c>
-      <c r="I43" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="J43" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="K43" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="L43" s="45"/>
-      <c r="M43" s="48" t="s">
-        <v>73</v>
+      <c r="M43" s="59" t="s">
+        <v>62</v>
       </c>
       <c r="N43" s="48"/>
       <c r="O43" s="47" t="s">
-        <v>212</v>
-      </c>
-      <c r="P43" s="46" t="s">
+        <v>305</v>
+      </c>
+      <c r="P43" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q43" s="63">
+        <v>6</v>
+      </c>
+      <c r="R43" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="S43" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="T43" s="64" t="s">
+        <v>312</v>
+      </c>
+      <c r="U43" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="32"/>
+      <c r="G44" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="H44" s="36">
+        <v>40</v>
+      </c>
+      <c r="I44" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="J44" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="K44" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L44" s="45"/>
+      <c r="M44" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="N44" s="48"/>
+      <c r="O44" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="P44" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="Q43" s="1">
+      <c r="Q44" s="1">
         <v>6</v>
       </c>
-      <c r="R43" s="13" t="s">
+      <c r="R44" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="S43" s="13" t="s">
+      <c r="S44" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="T43" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="U43" s="2" t="s">
+      <c r="T44" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="U44" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A44" s="18" t="s">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B45" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
-      <c r="O44" s="47"/>
-      <c r="P44" s="46"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="13"/>
-      <c r="S44" s="13"/>
-      <c r="T44" s="13"/>
-      <c r="U44" s="2"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A45" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="20" t="s">
         <v>91</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E45" s="31" t="s">
-        <v>111</v>
-      </c>
+      <c r="E45" s="31"/>
       <c r="F45" s="32"/>
-      <c r="G45" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="H45" s="36">
-        <v>41</v>
-      </c>
-      <c r="I45" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="J45" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="K45" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="L45" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="M45" s="48" t="s">
-        <v>50</v>
-      </c>
+      <c r="G45" s="38"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="45"/>
+      <c r="M45" s="48"/>
       <c r="N45" s="48"/>
-      <c r="O45" s="47" t="s">
-        <v>213</v>
-      </c>
-      <c r="P45" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q45" s="1">
-        <v>6</v>
-      </c>
-      <c r="R45" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="S45" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="T45" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
-      <c r="A46" s="18" t="s">
+      <c r="O45" s="47"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="2"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="24" t="s">
         <v>91</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>110</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F46" s="32"/>
       <c r="G46" s="38" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="H46" s="36">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I46" s="39" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="J46" s="37" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="K46" s="44" t="s">
         <v>69</v>
       </c>
       <c r="L46" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48" t="s">
-        <v>46</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M46" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="N46" s="48"/>
       <c r="O46" s="47" t="s">
-        <v>281</v>
+        <v>211</v>
       </c>
       <c r="P46" s="46" t="s">
         <v>19</v>
@@ -4476,59 +4564,59 @@
         <v>6</v>
       </c>
       <c r="R46" s="13" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="S46" s="13" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="T46" s="13" t="s">
-        <v>264</v>
+        <v>192</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A47" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="23" t="s">
+      <c r="B47" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="20" t="s">
         <v>91</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>110</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F47" s="32"/>
       <c r="G47" s="38" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="H47" s="36">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I47" s="39" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="J47" s="37" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="K47" s="44" t="s">
         <v>69</v>
       </c>
       <c r="L47" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="M47" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="N47" s="48"/>
+        <v>31</v>
+      </c>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48" t="s">
+        <v>46</v>
+      </c>
       <c r="O47" s="47" t="s">
-        <v>203</v>
+        <v>274</v>
       </c>
       <c r="P47" s="46" t="s">
         <v>19</v>
@@ -4537,74 +4625,80 @@
         <v>6</v>
       </c>
       <c r="R47" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="S47" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="T47" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="U47" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="86" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" s="88"/>
+      <c r="G48" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="H48" s="71">
+        <v>43</v>
+      </c>
+      <c r="I48" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="J48" s="73" t="s">
+        <v>243</v>
+      </c>
+      <c r="K48" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="L48" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="M48" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="N48" s="75"/>
+      <c r="O48" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="P48" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q48" s="63">
+        <v>6</v>
+      </c>
+      <c r="R48" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="S47" s="13" t="s">
+      <c r="S48" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="T47" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="U47" s="2" t="s">
+      <c r="T48" s="64" t="s">
+        <v>314</v>
+      </c>
+      <c r="U48" s="65" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A48" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="H48" s="36">
-        <v>44</v>
-      </c>
-      <c r="I48" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="J48" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="K48" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="L48" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="M48" s="48"/>
-      <c r="N48" s="48"/>
-      <c r="O48" s="47"/>
-      <c r="P48" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q48" s="49" t="s">
-        <v>151</v>
-      </c>
-      <c r="R48" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="S48" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="T48" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="U48" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>68</v>
       </c>
@@ -4620,16 +4714,16 @@
       <c r="E49" s="31"/>
       <c r="F49" s="32"/>
       <c r="G49" s="38" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H49" s="36">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I49" s="39" t="s">
         <v>125</v>
       </c>
       <c r="J49" s="37" t="s">
-        <v>249</v>
+        <v>195</v>
       </c>
       <c r="K49" s="44" t="s">
         <v>70</v>
@@ -4639,29 +4733,27 @@
       </c>
       <c r="M49" s="48"/>
       <c r="N49" s="48"/>
-      <c r="O49" s="47" t="s">
-        <v>172</v>
-      </c>
+      <c r="O49" s="47"/>
       <c r="P49" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q49" s="1">
-        <v>6</v>
+      <c r="Q49" s="49" t="s">
+        <v>151</v>
       </c>
       <c r="R49" s="13" t="s">
         <v>122</v>
       </c>
       <c r="S49" s="13" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="T49" s="13" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>68</v>
       </c>
@@ -4677,29 +4769,27 @@
       <c r="E50" s="31"/>
       <c r="F50" s="32"/>
       <c r="G50" s="38" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H50" s="36">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I50" s="39" t="s">
         <v>125</v>
       </c>
       <c r="J50" s="37" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="K50" s="44" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L50" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="M50" s="48" t="s">
-        <v>64</v>
-      </c>
+      <c r="M50" s="48"/>
       <c r="N50" s="48"/>
       <c r="O50" s="47" t="s">
-        <v>265</v>
+        <v>172</v>
       </c>
       <c r="P50" s="46" t="s">
         <v>19</v>
@@ -4708,19 +4798,19 @@
         <v>6</v>
       </c>
       <c r="R50" s="13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="S50" s="13" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="T50" s="13" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="28.65" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
         <v>68</v>
       </c>
@@ -4736,16 +4826,16 @@
       <c r="E51" s="31"/>
       <c r="F51" s="32"/>
       <c r="G51" s="38" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H51" s="36">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I51" s="39" t="s">
         <v>125</v>
       </c>
       <c r="J51" s="37" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="K51" s="44" t="s">
         <v>69</v>
@@ -4754,11 +4844,11 @@
         <v>32</v>
       </c>
       <c r="M51" s="48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N51" s="48"/>
       <c r="O51" s="47" t="s">
-        <v>223</v>
+        <v>260</v>
       </c>
       <c r="P51" s="46" t="s">
         <v>19</v>
@@ -4772,57 +4862,73 @@
       <c r="S51" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="T51" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="U51" s="4" t="s">
+      <c r="T51" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="U51" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A52" s="22" t="s">
+    <row r="52" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="D52" s="25" t="s">
-        <v>114</v>
+      <c r="D52" s="86" t="s">
+        <v>113</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="32"/>
-      <c r="G52" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="H52" s="36">
-        <v>48</v>
-      </c>
-      <c r="I52" s="39" t="s">
+      <c r="G52" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="H52" s="71">
+        <v>47</v>
+      </c>
+      <c r="I52" s="72" t="s">
         <v>125</v>
       </c>
-      <c r="J52" s="37" t="s">
-        <v>262</v>
-      </c>
-      <c r="K52" s="44" t="s">
+      <c r="J52" s="73" t="s">
+        <v>267</v>
+      </c>
+      <c r="K52" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L52" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="M52" s="48"/>
+      <c r="L52" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="M52" s="75" t="s">
+        <v>62</v>
+      </c>
       <c r="N52" s="48"/>
-      <c r="O52" s="47"/>
-      <c r="P52" s="46"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="13"/>
-      <c r="S52" s="13"/>
-      <c r="T52" s="13"/>
-      <c r="U52" s="2"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="O52" s="60" t="s">
+        <v>318</v>
+      </c>
+      <c r="P52" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q52" s="63">
+        <v>6</v>
+      </c>
+      <c r="R52" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="S52" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="T52" s="82" t="s">
+        <v>319</v>
+      </c>
+      <c r="U52" s="82" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
         <v>68</v>
       </c>
@@ -4833,51 +4939,39 @@
         <v>91</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E53" s="31"/>
       <c r="F53" s="32"/>
       <c r="G53" s="38" t="s">
-        <v>115</v>
+        <v>206</v>
       </c>
       <c r="H53" s="36">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I53" s="39" t="s">
         <v>125</v>
       </c>
       <c r="J53" s="37" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="K53" s="44" t="s">
         <v>69</v>
       </c>
       <c r="L53" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="M53" s="48" t="s">
-        <v>23</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="M53" s="48"/>
       <c r="N53" s="48"/>
       <c r="O53" s="47"/>
       <c r="P53" s="46"/>
-      <c r="Q53" s="1">
-        <v>6</v>
-      </c>
-      <c r="R53" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="S53" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="T53" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="U53" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="Q53" s="1"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="13"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="2"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
         <v>68</v>
       </c>
@@ -4888,23 +4982,41 @@
         <v>91</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>308</v>
+        <v>115</v>
       </c>
       <c r="E54" s="31"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="44"/>
-      <c r="L54" s="45"/>
+      <c r="G54" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="H54" s="36">
+        <v>49</v>
+      </c>
+      <c r="I54" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="J54" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="K54" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="L54" s="45" t="s">
+        <v>32</v>
+      </c>
       <c r="M54" s="48" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="N54" s="48"/>
-      <c r="O54" s="47"/>
-      <c r="P54" s="46"/>
-      <c r="Q54" s="1"/>
+      <c r="O54" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="P54" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>6</v>
+      </c>
       <c r="R54" s="13" t="s">
         <v>126</v>
       </c>
@@ -4912,43 +5024,73 @@
         <v>127</v>
       </c>
       <c r="T54" s="13" t="s">
-        <v>128</v>
+        <v>207</v>
       </c>
       <c r="U54" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A55" s="22"/>
-      <c r="B55" s="23"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="25"/>
+    <row r="55" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" s="86" t="s">
+        <v>300</v>
+      </c>
       <c r="E55" s="31"/>
       <c r="F55" s="32"/>
       <c r="G55" s="41"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="44"/>
-      <c r="L55" s="45"/>
-      <c r="M55" s="48"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="J55" s="73" t="s">
+        <v>315</v>
+      </c>
+      <c r="K55" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="L55" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="M55" s="75" t="s">
+        <v>63</v>
+      </c>
       <c r="N55" s="48"/>
-      <c r="O55" s="47"/>
+      <c r="O55" s="60" t="s">
+        <v>316</v>
+      </c>
       <c r="P55" s="46"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="13"/>
-      <c r="S55" s="13"/>
-      <c r="T55" s="13"/>
-      <c r="U55" s="2"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="Q55" s="63">
+        <v>6</v>
+      </c>
+      <c r="R55" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="S55" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="T55" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="U55" s="65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="22"/>
       <c r="B56" s="23"/>
       <c r="C56" s="24"/>
       <c r="D56" s="25"/>
       <c r="E56" s="31"/>
       <c r="F56" s="32"/>
-      <c r="G56" s="38"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="39"/>
       <c r="I56" s="39"/>
       <c r="J56" s="40"/>
@@ -4964,7 +5106,7 @@
       <c r="T56" s="13"/>
       <c r="U56" s="2"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
       <c r="B57" s="23"/>
       <c r="C57" s="24"/>
@@ -4987,7 +5129,7 @@
       <c r="T57" s="13"/>
       <c r="U57" s="2"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
       <c r="B58" s="23"/>
       <c r="C58" s="24"/>
@@ -5010,7 +5152,7 @@
       <c r="T58" s="13"/>
       <c r="U58" s="2"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
       <c r="B59" s="23"/>
       <c r="C59" s="24"/>
@@ -5033,7 +5175,7 @@
       <c r="T59" s="13"/>
       <c r="U59" s="2"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
       <c r="B60" s="23"/>
       <c r="C60" s="24"/>
@@ -5056,7 +5198,7 @@
       <c r="T60" s="13"/>
       <c r="U60" s="2"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="23"/>
       <c r="C61" s="24"/>
@@ -5066,7 +5208,7 @@
       <c r="G61" s="38"/>
       <c r="H61" s="39"/>
       <c r="I61" s="39"/>
-      <c r="J61" s="37"/>
+      <c r="J61" s="40"/>
       <c r="K61" s="44"/>
       <c r="L61" s="45"/>
       <c r="M61" s="48"/>
@@ -5079,7 +5221,7 @@
       <c r="T61" s="13"/>
       <c r="U61" s="2"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
       <c r="B62" s="23"/>
       <c r="C62" s="24"/>
@@ -5089,7 +5231,7 @@
       <c r="G62" s="38"/>
       <c r="H62" s="39"/>
       <c r="I62" s="39"/>
-      <c r="J62" s="40"/>
+      <c r="J62" s="37"/>
       <c r="K62" s="44"/>
       <c r="L62" s="45"/>
       <c r="M62" s="48"/>
@@ -5102,7 +5244,7 @@
       <c r="T62" s="13"/>
       <c r="U62" s="2"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="22"/>
       <c r="B63" s="23"/>
       <c r="C63" s="24"/>
@@ -5125,7 +5267,7 @@
       <c r="T63" s="13"/>
       <c r="U63" s="2"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="22"/>
       <c r="B64" s="23"/>
       <c r="C64" s="24"/>
@@ -5148,7 +5290,7 @@
       <c r="T64" s="13"/>
       <c r="U64" s="2"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="22"/>
       <c r="B65" s="23"/>
       <c r="C65" s="24"/>
@@ -5171,7 +5313,7 @@
       <c r="T65" s="13"/>
       <c r="U65" s="2"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="22"/>
       <c r="B66" s="23"/>
       <c r="C66" s="24"/>
@@ -5194,7 +5336,7 @@
       <c r="T66" s="13"/>
       <c r="U66" s="2"/>
     </row>
-    <row r="67" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="22"/>
       <c r="B67" s="23"/>
       <c r="C67" s="24"/>
@@ -5217,7 +5359,7 @@
       <c r="T67" s="13"/>
       <c r="U67" s="2"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22"/>
       <c r="B68" s="23"/>
       <c r="C68" s="24"/>
@@ -5240,7 +5382,7 @@
       <c r="T68" s="13"/>
       <c r="U68" s="2"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="22"/>
       <c r="B69" s="23"/>
       <c r="C69" s="24"/>
@@ -5263,7 +5405,7 @@
       <c r="T69" s="13"/>
       <c r="U69" s="2"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="22"/>
       <c r="B70" s="23"/>
       <c r="C70" s="24"/>
@@ -5286,13 +5428,13 @@
       <c r="T70" s="13"/>
       <c r="U70" s="2"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="22"/>
       <c r="B71" s="23"/>
       <c r="C71" s="24"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="33"/>
-      <c r="F71" s="34"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="32"/>
       <c r="G71" s="38"/>
       <c r="H71" s="39"/>
       <c r="I71" s="39"/>
@@ -5309,7 +5451,7 @@
       <c r="T71" s="13"/>
       <c r="U71" s="2"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="22"/>
       <c r="B72" s="23"/>
       <c r="C72" s="24"/>
@@ -5332,7 +5474,7 @@
       <c r="T72" s="13"/>
       <c r="U72" s="2"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="22"/>
       <c r="B73" s="23"/>
       <c r="C73" s="24"/>
@@ -5355,7 +5497,7 @@
       <c r="T73" s="13"/>
       <c r="U73" s="2"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="22"/>
       <c r="B74" s="23"/>
       <c r="C74" s="24"/>
@@ -5378,7 +5520,7 @@
       <c r="T74" s="13"/>
       <c r="U74" s="2"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="22"/>
       <c r="B75" s="23"/>
       <c r="C75" s="24"/>
@@ -5401,7 +5543,7 @@
       <c r="T75" s="13"/>
       <c r="U75" s="2"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
       <c r="B76" s="23"/>
       <c r="C76" s="24"/>
@@ -5424,7 +5566,7 @@
       <c r="T76" s="13"/>
       <c r="U76" s="2"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="22"/>
       <c r="B77" s="23"/>
       <c r="C77" s="24"/>
@@ -5447,7 +5589,7 @@
       <c r="T77" s="13"/>
       <c r="U77" s="2"/>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="22"/>
       <c r="B78" s="23"/>
       <c r="C78" s="24"/>
@@ -5470,7 +5612,7 @@
       <c r="T78" s="13"/>
       <c r="U78" s="2"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="22"/>
       <c r="B79" s="23"/>
       <c r="C79" s="24"/>
@@ -5493,7 +5635,7 @@
       <c r="T79" s="13"/>
       <c r="U79" s="2"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
       <c r="B80" s="23"/>
       <c r="C80" s="24"/>
@@ -5516,7 +5658,7 @@
       <c r="T80" s="13"/>
       <c r="U80" s="2"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="22"/>
       <c r="B81" s="23"/>
       <c r="C81" s="24"/>
@@ -5539,7 +5681,7 @@
       <c r="T81" s="13"/>
       <c r="U81" s="2"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="22"/>
       <c r="B82" s="23"/>
       <c r="C82" s="24"/>
@@ -5562,7 +5704,7 @@
       <c r="T82" s="13"/>
       <c r="U82" s="2"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
       <c r="B83" s="23"/>
       <c r="C83" s="24"/>
@@ -5585,7 +5727,7 @@
       <c r="T83" s="13"/>
       <c r="U83" s="2"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
       <c r="B84" s="23"/>
       <c r="C84" s="24"/>
@@ -5608,7 +5750,7 @@
       <c r="T84" s="13"/>
       <c r="U84" s="2"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="22"/>
       <c r="B85" s="23"/>
       <c r="C85" s="24"/>
@@ -5631,7 +5773,7 @@
       <c r="T85" s="13"/>
       <c r="U85" s="2"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
       <c r="B86" s="23"/>
       <c r="C86" s="24"/>
@@ -5654,7 +5796,7 @@
       <c r="T86" s="13"/>
       <c r="U86" s="2"/>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
       <c r="B87" s="23"/>
       <c r="C87" s="24"/>
@@ -5677,7 +5819,7 @@
       <c r="T87" s="13"/>
       <c r="U87" s="2"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="22"/>
       <c r="B88" s="23"/>
       <c r="C88" s="24"/>
@@ -5700,7 +5842,7 @@
       <c r="T88" s="13"/>
       <c r="U88" s="2"/>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="22"/>
       <c r="B89" s="23"/>
       <c r="C89" s="24"/>
@@ -5723,7 +5865,7 @@
       <c r="T89" s="13"/>
       <c r="U89" s="2"/>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="22"/>
       <c r="B90" s="23"/>
       <c r="C90" s="24"/>
@@ -5746,7 +5888,7 @@
       <c r="T90" s="13"/>
       <c r="U90" s="2"/>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="22"/>
       <c r="B91" s="23"/>
       <c r="C91" s="24"/>
@@ -5769,7 +5911,7 @@
       <c r="T91" s="13"/>
       <c r="U91" s="2"/>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="22"/>
       <c r="B92" s="23"/>
       <c r="C92" s="24"/>
@@ -5792,7 +5934,7 @@
       <c r="T92" s="13"/>
       <c r="U92" s="2"/>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="22"/>
       <c r="B93" s="23"/>
       <c r="C93" s="24"/>
@@ -5815,7 +5957,7 @@
       <c r="T93" s="13"/>
       <c r="U93" s="2"/>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="22"/>
       <c r="B94" s="23"/>
       <c r="C94" s="24"/>
@@ -5838,7 +5980,7 @@
       <c r="T94" s="13"/>
       <c r="U94" s="2"/>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="22"/>
       <c r="B95" s="23"/>
       <c r="C95" s="24"/>
@@ -5861,7 +6003,7 @@
       <c r="T95" s="13"/>
       <c r="U95" s="2"/>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="22"/>
       <c r="B96" s="23"/>
       <c r="C96" s="24"/>
@@ -5884,7 +6026,7 @@
       <c r="T96" s="13"/>
       <c r="U96" s="2"/>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="22"/>
       <c r="B97" s="23"/>
       <c r="C97" s="24"/>
@@ -5907,7 +6049,7 @@
       <c r="T97" s="13"/>
       <c r="U97" s="2"/>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="22"/>
       <c r="B98" s="23"/>
       <c r="C98" s="24"/>
@@ -5930,7 +6072,7 @@
       <c r="T98" s="13"/>
       <c r="U98" s="2"/>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="22"/>
       <c r="B99" s="23"/>
       <c r="C99" s="24"/>
@@ -5953,7 +6095,7 @@
       <c r="T99" s="13"/>
       <c r="U99" s="2"/>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="22"/>
       <c r="B100" s="23"/>
       <c r="C100" s="24"/>
@@ -5976,7 +6118,7 @@
       <c r="T100" s="13"/>
       <c r="U100" s="2"/>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="22"/>
       <c r="B101" s="23"/>
       <c r="C101" s="24"/>
@@ -5999,7 +6141,7 @@
       <c r="T101" s="13"/>
       <c r="U101" s="2"/>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="22"/>
       <c r="B102" s="23"/>
       <c r="C102" s="24"/>
@@ -6022,7 +6164,7 @@
       <c r="T102" s="13"/>
       <c r="U102" s="2"/>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="22"/>
       <c r="B103" s="23"/>
       <c r="C103" s="24"/>
@@ -6045,7 +6187,7 @@
       <c r="T103" s="13"/>
       <c r="U103" s="2"/>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="22"/>
       <c r="B104" s="23"/>
       <c r="C104" s="24"/>
@@ -6068,7 +6210,7 @@
       <c r="T104" s="13"/>
       <c r="U104" s="2"/>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="22"/>
       <c r="B105" s="23"/>
       <c r="C105" s="24"/>
@@ -6091,7 +6233,7 @@
       <c r="T105" s="13"/>
       <c r="U105" s="2"/>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="22"/>
       <c r="B106" s="23"/>
       <c r="C106" s="24"/>
@@ -6114,7 +6256,7 @@
       <c r="T106" s="13"/>
       <c r="U106" s="2"/>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="22"/>
       <c r="B107" s="23"/>
       <c r="C107" s="24"/>
@@ -6137,7 +6279,7 @@
       <c r="T107" s="13"/>
       <c r="U107" s="2"/>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="22"/>
       <c r="B108" s="23"/>
       <c r="C108" s="24"/>
@@ -6160,7 +6302,7 @@
       <c r="T108" s="13"/>
       <c r="U108" s="2"/>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="22"/>
       <c r="B109" s="23"/>
       <c r="C109" s="24"/>
@@ -6183,7 +6325,7 @@
       <c r="T109" s="13"/>
       <c r="U109" s="2"/>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="22"/>
       <c r="B110" s="23"/>
       <c r="C110" s="24"/>
@@ -6206,7 +6348,7 @@
       <c r="T110" s="13"/>
       <c r="U110" s="2"/>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" s="22"/>
       <c r="B111" s="23"/>
       <c r="C111" s="24"/>
@@ -6229,7 +6371,7 @@
       <c r="T111" s="13"/>
       <c r="U111" s="2"/>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="22"/>
       <c r="B112" s="23"/>
       <c r="C112" s="24"/>
@@ -6252,7 +6394,7 @@
       <c r="T112" s="13"/>
       <c r="U112" s="2"/>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="22"/>
       <c r="B113" s="23"/>
       <c r="C113" s="24"/>
@@ -6275,7 +6417,7 @@
       <c r="T113" s="13"/>
       <c r="U113" s="2"/>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="22"/>
       <c r="B114" s="23"/>
       <c r="C114" s="24"/>
@@ -6298,7 +6440,7 @@
       <c r="T114" s="13"/>
       <c r="U114" s="2"/>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="22"/>
       <c r="B115" s="23"/>
       <c r="C115" s="24"/>
@@ -6321,7 +6463,7 @@
       <c r="T115" s="13"/>
       <c r="U115" s="2"/>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="22"/>
       <c r="B116" s="23"/>
       <c r="C116" s="24"/>
@@ -6343,6 +6485,29 @@
       <c r="S116" s="13"/>
       <c r="T116" s="13"/>
       <c r="U116" s="2"/>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A117" s="22"/>
+      <c r="B117" s="23"/>
+      <c r="C117" s="24"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="33"/>
+      <c r="F117" s="34"/>
+      <c r="G117" s="38"/>
+      <c r="H117" s="39"/>
+      <c r="I117" s="39"/>
+      <c r="J117" s="40"/>
+      <c r="K117" s="44"/>
+      <c r="L117" s="45"/>
+      <c r="M117" s="48"/>
+      <c r="N117" s="48"/>
+      <c r="O117" s="47"/>
+      <c r="P117" s="46"/>
+      <c r="Q117" s="1"/>
+      <c r="R117" s="13"/>
+      <c r="S117" s="13"/>
+      <c r="T117" s="13"/>
+      <c r="U117" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -6376,37 +6541,37 @@
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N49 N51:N116</xm:sqref>
+          <xm:sqref>N3:N50 N52:N117</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K116</xm:sqref>
+          <xm:sqref>K3:K117</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L116</xm:sqref>
+          <xm:sqref>L3:L117</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P116</xm:sqref>
+          <xm:sqref>P3:P117</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M116</xm:sqref>
+          <xm:sqref>M3:M117</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A116</xm:sqref>
+          <xm:sqref>A3:A117</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6422,16 +6587,16 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -6454,7 +6619,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
         <v>34</v>
@@ -6475,7 +6640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="15" t="s">
         <v>35</v>
@@ -6496,7 +6661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="15" t="s">
         <v>36</v>
@@ -6513,7 +6678,7 @@
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="15" t="s">
         <v>37</v>
@@ -6530,7 +6695,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="15" t="s">
         <v>38</v>
@@ -6545,7 +6710,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="15" t="s">
         <v>39</v>
@@ -6558,7 +6723,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="15" t="s">
         <v>40</v>
@@ -6571,7 +6736,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="15" t="s">
         <v>41</v>
@@ -6584,7 +6749,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="15" t="s">
         <v>42</v>
@@ -6597,7 +6762,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="15" t="s">
         <v>43</v>
@@ -6612,7 +6777,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="15" t="s">
         <v>44</v>
@@ -6627,7 +6792,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15" t="s">
         <v>45</v>
@@ -6642,7 +6807,7 @@
       <c r="M13" s="6"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="15" t="s">
         <v>46</v>
@@ -6657,7 +6822,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15" t="s">
@@ -6670,7 +6835,7 @@
       <c r="M15" s="6"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
@@ -6683,7 +6848,7 @@
       <c r="M16" s="6"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15" t="s">
@@ -6696,7 +6861,7 @@
       <c r="M17" s="6"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
@@ -6709,7 +6874,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
@@ -6722,7 +6887,7 @@
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15" t="s">
@@ -6735,7 +6900,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
@@ -6748,7 +6913,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
@@ -6761,7 +6926,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15" t="s">
@@ -6774,7 +6939,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15" t="s">
@@ -6787,7 +6952,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15" t="s">
@@ -6798,7 +6963,7 @@
       <c r="F25" s="15"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
@@ -6809,7 +6974,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15" t="s">
@@ -6820,7 +6985,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15" t="s">
@@ -6831,7 +6996,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
@@ -6842,7 +7007,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15" t="s">
@@ -6853,7 +7018,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15" t="s">
@@ -6864,7 +7029,7 @@
       <c r="F31" s="15"/>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15" t="s">
@@ -6875,7 +7040,7 @@
       <c r="F32" s="15"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
@@ -6886,7 +7051,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
@@ -6897,7 +7062,7 @@
       <c r="F34" s="15"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15" t="s">
@@ -6908,7 +7073,7 @@
       <c r="F35" s="15"/>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15" t="s">
@@ -6919,7 +7084,7 @@
       <c r="F36" s="15"/>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="15" t="s">
@@ -6930,7 +7095,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11" t="s">
@@ -6941,7 +7106,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11" t="s">
@@ -6952,7 +7117,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -6961,7 +7126,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -6970,7 +7135,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -6979,7 +7144,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -6988,7 +7153,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -6997,7 +7162,7 @@
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -7006,7 +7171,7 @@
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -7015,7 +7180,7 @@
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -7024,7 +7189,7 @@
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -7033,7 +7198,7 @@
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -7042,7 +7207,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>

</xml_diff>

<commit_message>
Subida la guía didáctica del guion 1 de grado sexto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion01/Escaleta_LE_06_01_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion01/Escaleta_LE_06_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Lenguaje\fuentes\contenidos\grado06\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csepulveda\Desktop\GITHUB2015\Lenguaje\fuentes\contenidos\grado06\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1837,35 +1837,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U53" sqref="U53"/>
+    <sheetView tabSelected="1" topLeftCell="K8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.46484375" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.46484375" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.06640625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="26.1328125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" style="18" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="18" customWidth="1"/>
     <col min="6" max="6" width="15" style="18" customWidth="1"/>
-    <col min="7" max="7" width="53.86328125" style="18" customWidth="1"/>
-    <col min="8" max="9" width="5.86328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="51.19921875" style="18" customWidth="1"/>
-    <col min="11" max="12" width="10.6640625" style="70" customWidth="1"/>
-    <col min="13" max="13" width="8.19921875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="8.19921875" style="70" customWidth="1"/>
-    <col min="15" max="15" width="20.1328125" style="18" customWidth="1"/>
-    <col min="16" max="16" width="5.73046875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="6.86328125" style="18" customWidth="1"/>
-    <col min="18" max="18" width="5.73046875" style="18" customWidth="1"/>
-    <col min="19" max="19" width="14.73046875" style="18" customWidth="1"/>
-    <col min="20" max="20" width="23.1328125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="53.85546875" style="18" customWidth="1"/>
+    <col min="8" max="9" width="5.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="51.140625" style="18" customWidth="1"/>
+    <col min="11" max="12" width="10.7109375" style="70" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="18" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="70" customWidth="1"/>
+    <col min="15" max="15" width="143.5703125" style="18" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" style="18" customWidth="1"/>
+    <col min="18" max="18" width="5.7109375" style="18" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="18" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" style="18" customWidth="1"/>
     <col min="21" max="21" width="14" style="18" customWidth="1"/>
-    <col min="22" max="16384" width="10.6640625" style="18"/>
+    <col min="22" max="16384" width="10.7109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="20" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:21" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="72"/>
       <c r="B2" s="72"/>
       <c r="C2" s="72"/>
@@ -1955,7 +1955,7 @@
       <c r="T2" s="72"/>
       <c r="U2" s="72"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>68</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>68</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>68</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>68</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>68</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>68</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>68</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>68</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>68</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
         <v>68</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
         <v>68</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
         <v>68</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
         <v>68</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="51" t="s">
         <v>68</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="51" t="s">
         <v>68</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="51" t="s">
         <v>68</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="51" t="s">
         <v>68</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="51" t="s">
         <v>68</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
         <v>68</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="51" t="s">
         <v>68</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="51" t="s">
         <v>68</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
         <v>68</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
         <v>68</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="57" t="s">
         <v>68</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="51" t="s">
         <v>68</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>68</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
         <v>68</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>68</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="51" t="s">
         <v>68</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>68</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="51" t="s">
         <v>68</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="51" t="s">
         <v>68</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="51" t="s">
         <v>68</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="51" t="s">
         <v>68</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="51" t="s">
         <v>68</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="57" t="s">
         <v>68</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="51" t="s">
         <v>68</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="51" t="s">
         <v>68</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="51" t="s">
         <v>68</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="51" t="s">
         <v>68</v>
       </c>
@@ -4347,7 +4347,7 @@
       <c r="T42" s="5"/>
       <c r="U42" s="55"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
         <v>68</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="51" t="s">
         <v>68</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>68</v>
       </c>
@@ -4498,7 +4498,7 @@
       <c r="T45" s="5"/>
       <c r="U45" s="55"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="51" t="s">
         <v>68</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>68</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="57" t="s">
         <v>68</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="51" t="s">
         <v>68</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="51" t="s">
         <v>68</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="51" t="s">
         <v>68</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="57" t="s">
         <v>68</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="51" t="s">
         <v>68</v>
       </c>
@@ -4954,7 +4954,7 @@
       <c r="T53" s="5"/>
       <c r="U53" s="55"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="51" t="s">
         <v>68</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="57" t="s">
         <v>68</v>
       </c>
@@ -5075,11 +5075,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -5095,6 +5090,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5151,16 +5151,16 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>34</v>
@@ -5204,7 +5204,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>35</v>
@@ -5225,7 +5225,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>36</v>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>37</v>
@@ -5259,7 +5259,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>38</v>
@@ -5274,7 +5274,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>39</v>
@@ -5287,7 +5287,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
         <v>40</v>
@@ -5300,7 +5300,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
         <v>41</v>
@@ -5313,7 +5313,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7" t="s">
         <v>42</v>
@@ -5326,7 +5326,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
         <v>43</v>
@@ -5341,7 +5341,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
         <v>44</v>
@@ -5356,7 +5356,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
         <v>45</v>
@@ -5371,7 +5371,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
         <v>46</v>
@@ -5386,7 +5386,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
@@ -5399,7 +5399,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
@@ -5412,7 +5412,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
@@ -5425,7 +5425,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
@@ -5438,7 +5438,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
@@ -5451,7 +5451,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
@@ -5464,7 +5464,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
@@ -5477,7 +5477,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
@@ -5490,7 +5490,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
@@ -5503,7 +5503,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
@@ -5516,7 +5516,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -5527,7 +5527,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
@@ -5538,7 +5538,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
@@ -5549,7 +5549,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
@@ -5560,7 +5560,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
@@ -5571,7 +5571,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
@@ -5582,7 +5582,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
@@ -5593,7 +5593,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
@@ -5604,7 +5604,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
@@ -5615,7 +5615,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
@@ -5626,7 +5626,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
@@ -5637,7 +5637,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
@@ -5648,7 +5648,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="7" t="s">
@@ -5659,7 +5659,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
@@ -5670,7 +5670,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
@@ -5681,7 +5681,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -5690,7 +5690,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -5699,7 +5699,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -5708,7 +5708,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -5717,7 +5717,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -5726,7 +5726,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -5735,7 +5735,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -5744,7 +5744,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -5753,7 +5753,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -5762,7 +5762,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -5771,7 +5771,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>

</xml_diff>

<commit_message>
Actualizado y entregado guion 1 de sexto y mapa conceptual de guion 1 de sexto los definitivos.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion01/Escaleta_LE_06_01_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion01/Escaleta_LE_06_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csepulveda\Desktop\GITHUB2015\Lenguaje\fuentes\contenidos\grado06\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csepulveda\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -628,9 +628,6 @@
     <t>Recurso M1D-02</t>
   </si>
   <si>
-    <t>Actividad diseñada para que el estudiante identifique el uso de las grafías “q” y “k” en las palabras y oraciones</t>
-  </si>
-  <si>
     <t>Recurso M2C-02</t>
   </si>
   <si>
@@ -670,9 +667,6 @@
     <t>Recurso M102AB-01</t>
   </si>
   <si>
-    <t>Este recurso busca que el estudiante reconozca palabras que se escriben con "q" y "k"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Este es un recurso completamente nuevo. La idea es presentar al estudiante algunas palabras, con imágenes, en las que se incluyan la "q" y la "k". </t>
   </si>
   <si>
@@ -766,33 +760,18 @@
     <t>Competencias: Escribe textos informativos</t>
   </si>
   <si>
-    <t>En este recurso el estudiante puede relacionar algunos textos con las partes de la narración</t>
-  </si>
-  <si>
     <t>Actividad que permite ejercitar la comprensión y producción de textos descriptivos con el uso de léxico específico</t>
   </si>
   <si>
-    <t>Actividad interactiva que le permite al estudiante reconocer prosas y mejorar su comprensión lectora</t>
-  </si>
-  <si>
     <t>En este recurso el estudiante aprenderá a identificar y medir la extensión de los versos</t>
   </si>
   <si>
-    <t>Con este recurso el estudiante puede abordar algunas características de las categorías gramaticales junto con los elementos que las componen</t>
-  </si>
-  <si>
     <t>Actividades de reconocimiento sobre las categorías gramaticales, especialmente sustantivos y adjetivos</t>
   </si>
   <si>
     <t xml:space="preserve">Actividad con la que se practica el reconocimiento de la grafía “q” a partir de la identificación de imágenes </t>
   </si>
   <si>
-    <t>Actividad para que los estudiantes reconozcan la estructura de un reportaje</t>
-  </si>
-  <si>
-    <t>Este recurso plantea la redacción de reportajes por parte de los estudiantes teniendo en cuenta su estructura</t>
-  </si>
-  <si>
     <t>Actividad para clasificar algunas palabras de acuerdo a su respectiva categoría gramatical</t>
   </si>
   <si>
@@ -808,24 +787,12 @@
     <t>Secuencia de diferentes imágenes que permiten un acercamiento a la literatura y el tipo de discurso que emplea</t>
   </si>
   <si>
-    <t>Actividad interactiva que le permite al estudiante acercarse a la redacción de diálogos y mejorar su comprensión lectora</t>
-  </si>
-  <si>
-    <t>Actividad interactiva que permite al estudiante practicar la lectura de versos</t>
-  </si>
-  <si>
     <t>Mediante este recurso el estudiante puede encontrar léxico apropiado para usar en descripciones</t>
   </si>
   <si>
-    <t>Actividad que permite al estudiante construir descripciones a partir de la formulación de preguntas claves</t>
-  </si>
-  <si>
     <t>Actividad para descubrir categorías gramaticales, especialmente adjetivos, de forma lúdica</t>
   </si>
   <si>
-    <t>Por medio de este recurso los estudiantes podrán hacer un ejercicio de escucha y clasificación de las categorías gramaticales estudiadas</t>
-  </si>
-  <si>
     <t>Actividad para hallar errores de ortografía relacionados con el empleo de la “q”</t>
   </si>
   <si>
@@ -835,9 +802,6 @@
     <t xml:space="preserve">Mapa conceptual del tema El reportaje </t>
   </si>
   <si>
-    <t>Actividad para evaluar los conocimientos del estudiante sobre el tema El reportaje</t>
-  </si>
-  <si>
     <t>Recurso F13B-01</t>
   </si>
   <si>
@@ -892,28 +856,10 @@
     <t>Los textos literarios y sus características</t>
   </si>
   <si>
-    <t>En este recurso el estudiante algunos rasgos que hacen que un texto sea literario</t>
-  </si>
-  <si>
     <t>Las categorías gramaticales: los sustantivos y los adjetivos</t>
   </si>
   <si>
-    <t>En este recurso el estudiante puede establecer relaciones entre las categorías gramaticales (sustantivo y adjetivo)  y su definición, incluyendo algunos ejemplos.</t>
-  </si>
-  <si>
     <t>El uso de palabras con "q" y "k"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esta es una actividad para que el estudiante recuerde la escritura correcta de palabras con "q" y "k" </t>
-  </si>
-  <si>
-    <t>Por medio de este recurso el estudiante puede organizar los textos que escucha de acuerdo a su intención comunicativa y tipología</t>
-  </si>
-  <si>
-    <t>Esta actividad permite que el estudiante señale algunas características de los textos informativos, especialmente de los reportajes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En esta actividad se busca que el estudiante proponga la manera en que organizaría la escritura de un reportaje (pasos) y las partes que tendría en cuenta </t>
   </si>
   <si>
     <t xml:space="preserve">La clasificación de textos de acuerdo a su intención comunicativa </t>
@@ -997,9 +943,6 @@
     <t>Ortografía: los grafemas q y k</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: analiza casos del uso de llos grafemas q y k </t>
-  </si>
-  <si>
     <t xml:space="preserve">Actividad para afianzar la práctica de las reglas ortográficas de los grafemas q y k </t>
   </si>
   <si>
@@ -1034,13 +977,70 @@
   </si>
   <si>
     <t>RM_01_02_CO</t>
+  </si>
+  <si>
+    <t>En este recurso se reconocen algunos rasgos que hacen que un texto sea literario</t>
+  </si>
+  <si>
+    <t>Actividad para establecer relaciones entre las categorías gramaticales (sustantivo y adjetivo) y su definición, incluyendo algunos ejemplos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para recordar la escritura correcta de palabras con q y k </t>
+  </si>
+  <si>
+    <t>Por medio de este recurso se pueden organizar los textos según su intención comunicativa y tipología</t>
+  </si>
+  <si>
+    <t>Esta actividad permite señalar algunas características de los textos informativos, especialmente de los reportajes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para determinar cómo organizar la escritura de un reportaje </t>
+  </si>
+  <si>
+    <t>En este recurso se identifican las partes de la narración en diferentes textos literarios</t>
+  </si>
+  <si>
+    <t>Actividad interactiva que permite practicar la lectura de versos</t>
+  </si>
+  <si>
+    <t>Actividad interactiva que permite reconocer prosas y mejorar la comprensión lectora</t>
+  </si>
+  <si>
+    <t>Actividad interactiva para la redacción de diálogos y el desarrollo de la comprensión lectora</t>
+  </si>
+  <si>
+    <t>Actividad que permite construir descripciones a partir de la formulación de preguntas clave</t>
+  </si>
+  <si>
+    <t>Con este recurso se abordan algunas características de las categorías gramaticales junto con los elementos que las componen</t>
+  </si>
+  <si>
+    <t>Por medio de este ejercicio de escucha se propone la clasificación de las categorías gramaticales estudiadas</t>
+  </si>
+  <si>
+    <t>Este recurso busca  que se reconozcan palabras que se escriben con q y k</t>
+  </si>
+  <si>
+    <t>Actividad diseñada para identificar el uso de las grafías q y k en las palabras y oraciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Analiza casos del uso de llos grafemas q y k </t>
+  </si>
+  <si>
+    <t>Actividad para reconocer la estructura de un reportaje</t>
+  </si>
+  <si>
+    <t>Este recurso plantea la redacción de reportajes teniendo en cuenta su estructura</t>
+  </si>
+  <si>
+    <t>Evalúa tus conocimientos sobre el tema El reportaje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1082,6 +1082,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1445,7 +1451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1555,6 +1561,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1837,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P60" sqref="P60"/>
+    <sheetView tabSelected="1" topLeftCell="E35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,7 +1978,7 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="26" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="H3" s="9">
         <v>1</v>
@@ -1980,7 +1987,7 @@
         <v>124</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="K3" s="28" t="s">
         <v>69</v>
@@ -1993,7 +2000,7 @@
         <v>84</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>19</v>
@@ -2008,7 +2015,7 @@
         <v>126</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U3" s="31" t="s">
         <v>128</v>
@@ -2030,7 +2037,7 @@
       <c r="E4" s="32"/>
       <c r="F4" s="25"/>
       <c r="G4" s="26" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -2039,7 +2046,7 @@
         <v>124</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="K4" s="28" t="s">
         <v>69</v>
@@ -2052,7 +2059,7 @@
         <v>73</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>19</v>
@@ -2067,7 +2074,7 @@
         <v>126</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="U4" s="31" t="s">
         <v>128</v>
@@ -2089,7 +2096,7 @@
       <c r="E5" s="32"/>
       <c r="F5" s="25"/>
       <c r="G5" s="26" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -2098,7 +2105,7 @@
         <v>124</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>69</v>
@@ -2111,7 +2118,7 @@
         <v>22</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>19</v>
@@ -2148,7 +2155,7 @@
       <c r="E6" s="32"/>
       <c r="F6" s="25"/>
       <c r="G6" s="26" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -2157,7 +2164,7 @@
         <v>124</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="K6" s="28" t="s">
         <v>69</v>
@@ -2170,7 +2177,7 @@
         <v>79</v>
       </c>
       <c r="O6" s="29" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>19</v>
@@ -2185,7 +2192,7 @@
         <v>126</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="U6" s="31" t="s">
         <v>128</v>
@@ -2207,7 +2214,7 @@
       <c r="E7" s="32"/>
       <c r="F7" s="25"/>
       <c r="G7" s="26" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -2216,7 +2223,7 @@
         <v>124</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="K7" s="28" t="s">
         <v>69</v>
@@ -2229,7 +2236,7 @@
         <v>24</v>
       </c>
       <c r="O7" s="29" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="P7" s="11" t="s">
         <v>19</v>
@@ -2244,7 +2251,7 @@
         <v>126</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="U7" s="31" t="s">
         <v>128</v>
@@ -2266,7 +2273,7 @@
       <c r="E8" s="36"/>
       <c r="F8" s="37"/>
       <c r="G8" s="38" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
@@ -2275,7 +2282,7 @@
         <v>124</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="K8" s="40" t="s">
         <v>69</v>
@@ -2288,7 +2295,7 @@
         <v>62</v>
       </c>
       <c r="O8" s="41" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="P8" s="16" t="s">
         <v>19</v>
@@ -2336,7 +2343,7 @@
         <v>119</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="K9" s="28" t="s">
         <v>70</v>
@@ -2347,7 +2354,7 @@
       <c r="M9" s="29"/>
       <c r="N9" s="29"/>
       <c r="O9" s="46" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>19</v>
@@ -2395,7 +2402,7 @@
         <v>124</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="K10" s="40" t="s">
         <v>69</v>
@@ -2408,7 +2415,7 @@
         <v>62</v>
       </c>
       <c r="O10" s="49" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="P10" s="16" t="s">
         <v>19</v>
@@ -2458,7 +2465,7 @@
         <v>124</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>234</v>
+        <v>307</v>
       </c>
       <c r="K11" s="53" t="s">
         <v>69</v>
@@ -2471,7 +2478,7 @@
         <v>61</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>19</v>
@@ -2521,7 +2528,7 @@
         <v>119</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="K12" s="53" t="s">
         <v>69</v>
@@ -2534,7 +2541,7 @@
       </c>
       <c r="N12" s="29"/>
       <c r="O12" s="46" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>19</v>
@@ -2595,7 +2602,7 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="46" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>19</v>
@@ -2695,7 +2702,7 @@
         <v>96</v>
       </c>
       <c r="G15" s="45" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2717,7 +2724,7 @@
         <v>77</v>
       </c>
       <c r="O15" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>19</v>
@@ -2797,7 +2804,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="51" t="s">
         <v>68</v>
       </c>
@@ -2825,8 +2832,8 @@
       <c r="I17" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="J17" s="27" t="s">
-        <v>248</v>
+      <c r="J17" s="77" t="s">
+        <v>310</v>
       </c>
       <c r="K17" s="53" t="s">
         <v>69</v>
@@ -2839,7 +2846,7 @@
       </c>
       <c r="N17" s="29"/>
       <c r="O17" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>19</v>
@@ -2948,7 +2955,7 @@
         <v>124</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="K19" s="53" t="s">
         <v>69</v>
@@ -2961,7 +2968,7 @@
         <v>22</v>
       </c>
       <c r="O19" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>19</v>
@@ -2976,7 +2983,7 @@
         <v>126</v>
       </c>
       <c r="T19" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U19" s="31" t="s">
         <v>128</v>
@@ -3011,7 +3018,7 @@
         <v>139</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>236</v>
+        <v>309</v>
       </c>
       <c r="K20" s="53" t="s">
         <v>69</v>
@@ -3024,7 +3031,7 @@
       </c>
       <c r="N20" s="29"/>
       <c r="O20" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>19</v>
@@ -3074,7 +3081,7 @@
         <v>124</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="K21" s="53" t="s">
         <v>69</v>
@@ -3087,7 +3094,7 @@
         <v>76</v>
       </c>
       <c r="O21" s="46" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P21" s="11" t="s">
         <v>19</v>
@@ -3137,7 +3144,7 @@
         <v>139</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>249</v>
+        <v>308</v>
       </c>
       <c r="K22" s="53" t="s">
         <v>69</v>
@@ -3150,7 +3157,7 @@
       </c>
       <c r="N22" s="29"/>
       <c r="O22" s="46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P22" s="11" t="s">
         <v>19</v>
@@ -3189,7 +3196,7 @@
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="45" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H23" s="9">
         <v>21</v>
@@ -3209,7 +3216,7 @@
       <c r="M23" s="29"/>
       <c r="N23" s="29"/>
       <c r="O23" s="46" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="P23" s="11" t="s">
         <v>19</v>
@@ -3248,7 +3255,7 @@
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H24" s="9">
         <v>22</v>
@@ -3305,7 +3312,7 @@
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="45" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H25" s="9">
         <v>23</v>
@@ -3314,7 +3321,7 @@
         <v>124</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="K25" s="53" t="s">
         <v>70</v>
@@ -3362,7 +3369,7 @@
       </c>
       <c r="F26" s="37"/>
       <c r="G26" s="48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H26" s="9">
         <v>24</v>
@@ -3371,7 +3378,7 @@
         <v>124</v>
       </c>
       <c r="J26" s="39" t="s">
-        <v>251</v>
+        <v>311</v>
       </c>
       <c r="K26" s="59" t="s">
         <v>69</v>
@@ -3384,7 +3391,7 @@
         <v>62</v>
       </c>
       <c r="O26" s="49" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="P26" s="11" t="s">
         <v>20</v>
@@ -3399,7 +3406,7 @@
         <v>126</v>
       </c>
       <c r="T26" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U26" s="61" t="s">
         <v>128</v>
@@ -3416,7 +3423,7 @@
         <v>91</v>
       </c>
       <c r="D27" s="62" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>102</v>
@@ -3432,7 +3439,7 @@
         <v>139</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>238</v>
+        <v>312</v>
       </c>
       <c r="K27" s="53" t="s">
         <v>69</v>
@@ -3445,7 +3452,7 @@
       </c>
       <c r="N27" s="29"/>
       <c r="O27" s="46" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P27" s="11" t="s">
         <v>19</v>
@@ -3552,7 +3559,7 @@
         <v>124</v>
       </c>
       <c r="J29" s="27" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="K29" s="53" t="s">
         <v>70</v>
@@ -3602,7 +3609,7 @@
       </c>
       <c r="F30" s="66"/>
       <c r="G30" s="48" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H30" s="9">
         <v>28</v>
@@ -3611,7 +3618,7 @@
         <v>124</v>
       </c>
       <c r="J30" s="39" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="K30" s="59" t="s">
         <v>69</v>
@@ -3624,7 +3631,7 @@
         <v>62</v>
       </c>
       <c r="O30" s="49" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="P30" s="16" t="s">
         <v>19</v>
@@ -3639,13 +3646,13 @@
         <v>126</v>
       </c>
       <c r="T30" s="13" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="U30" s="61" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="51" t="s">
         <v>68</v>
       </c>
@@ -3663,7 +3670,7 @@
       </c>
       <c r="F31" s="63"/>
       <c r="G31" s="45" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H31" s="9">
         <v>29</v>
@@ -3671,8 +3678,8 @@
       <c r="I31" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="J31" s="27" t="s">
-        <v>253</v>
+      <c r="J31" s="77" t="s">
+        <v>313</v>
       </c>
       <c r="K31" s="53" t="s">
         <v>69</v>
@@ -3685,7 +3692,7 @@
         <v>79</v>
       </c>
       <c r="O31" s="46" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P31" s="11" t="s">
         <v>19</v>
@@ -3700,7 +3707,7 @@
         <v>126</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="U31" s="55" t="s">
         <v>128</v>
@@ -3724,7 +3731,7 @@
       </c>
       <c r="F32" s="63"/>
       <c r="G32" s="45" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H32" s="9">
         <v>30</v>
@@ -3733,7 +3740,7 @@
         <v>139</v>
       </c>
       <c r="J32" s="68" t="s">
-        <v>202</v>
+        <v>314</v>
       </c>
       <c r="K32" s="53" t="s">
         <v>69</v>
@@ -3746,7 +3753,7 @@
       </c>
       <c r="N32" s="29"/>
       <c r="O32" s="46" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P32" s="11" t="s">
         <v>19</v>
@@ -3761,7 +3768,7 @@
         <v>132</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="U32" s="55" t="s">
         <v>134</v>
@@ -3794,7 +3801,7 @@
         <v>124</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="K33" s="53" t="s">
         <v>69</v>
@@ -3807,7 +3814,7 @@
         <v>47</v>
       </c>
       <c r="O33" s="46" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P33" s="11" t="s">
         <v>19</v>
@@ -3855,7 +3862,7 @@
         <v>124</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="K34" s="53" t="s">
         <v>69</v>
@@ -3868,7 +3875,7 @@
         <v>75</v>
       </c>
       <c r="O34" s="46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P34" s="11" t="s">
         <v>19</v>
@@ -3929,7 +3936,7 @@
         <v>60</v>
       </c>
       <c r="O35" s="46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P35" s="11" t="s">
         <v>19</v>
@@ -3977,7 +3984,7 @@
         <v>124</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="K36" s="53" t="s">
         <v>69</v>
@@ -3990,7 +3997,7 @@
         <v>75</v>
       </c>
       <c r="O36" s="46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P36" s="11"/>
       <c r="Q36" s="47">
@@ -4027,7 +4034,7 @@
       </c>
       <c r="F37" s="63"/>
       <c r="G37" s="45" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H37" s="9">
         <v>35</v>
@@ -4036,7 +4043,7 @@
         <v>124</v>
       </c>
       <c r="J37" s="27" t="s">
-        <v>188</v>
+        <v>315</v>
       </c>
       <c r="K37" s="53" t="s">
         <v>69</v>
@@ -4049,7 +4056,7 @@
         <v>22</v>
       </c>
       <c r="O37" s="46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P37" s="11" t="s">
         <v>19</v>
@@ -4064,7 +4071,7 @@
         <v>126</v>
       </c>
       <c r="T37" s="31" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="U37" s="31" t="s">
         <v>128</v>
@@ -4081,23 +4088,23 @@
         <v>91</v>
       </c>
       <c r="D38" s="64" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="E38" s="65" t="s">
         <v>101</v>
       </c>
       <c r="F38" s="63"/>
       <c r="G38" s="48" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="H38" s="9">
         <v>36</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J38" s="39" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="K38" s="59" t="s">
         <v>69</v>
@@ -4110,7 +4117,7 @@
         <v>62</v>
       </c>
       <c r="O38" s="49" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="P38" s="16" t="s">
         <v>19</v>
@@ -4122,10 +4129,10 @@
         <v>125</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="T38" s="69" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="U38" s="44" t="s">
         <v>128</v>
@@ -4149,16 +4156,16 @@
       </c>
       <c r="F39" s="63"/>
       <c r="G39" s="45" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H39" s="9">
         <v>37</v>
       </c>
       <c r="I39" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J39" s="27" t="s">
         <v>195</v>
-      </c>
-      <c r="J39" s="27" t="s">
-        <v>196</v>
       </c>
       <c r="K39" s="53" t="s">
         <v>69</v>
@@ -4171,7 +4178,7 @@
         <v>58</v>
       </c>
       <c r="O39" s="46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P39" s="11" t="s">
         <v>20</v>
@@ -4186,7 +4193,7 @@
         <v>126</v>
       </c>
       <c r="T39" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U39" s="55" t="s">
         <v>128</v>
@@ -4203,14 +4210,14 @@
         <v>91</v>
       </c>
       <c r="D40" s="62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E40" s="67" t="s">
         <v>106</v>
       </c>
       <c r="F40" s="63"/>
       <c r="G40" s="45" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="H40" s="9">
         <v>38</v>
@@ -4219,7 +4226,7 @@
         <v>139</v>
       </c>
       <c r="J40" s="27" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="K40" s="53" t="s">
         <v>69</v>
@@ -4232,7 +4239,7 @@
       </c>
       <c r="N40" s="29"/>
       <c r="O40" s="46" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="P40" s="11" t="s">
         <v>19</v>
@@ -4247,7 +4254,7 @@
         <v>132</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U40" s="55" t="s">
         <v>134</v>
@@ -4264,14 +4271,14 @@
         <v>91</v>
       </c>
       <c r="D41" s="62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E41" s="67" t="s">
         <v>107</v>
       </c>
       <c r="F41" s="63"/>
       <c r="G41" s="45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H41" s="9">
         <v>39</v>
@@ -4280,7 +4287,7 @@
         <v>124</v>
       </c>
       <c r="J41" s="27" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="K41" s="53" t="s">
         <v>69</v>
@@ -4293,7 +4300,7 @@
         <v>84</v>
       </c>
       <c r="O41" s="46" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="P41" s="11" t="s">
         <v>19</v>
@@ -4308,7 +4315,7 @@
         <v>126</v>
       </c>
       <c r="T41" s="5" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="U41" s="55" t="s">
         <v>128</v>
@@ -4325,7 +4332,7 @@
         <v>91</v>
       </c>
       <c r="D42" s="62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E42" s="67" t="s">
         <v>108</v>
@@ -4358,14 +4365,14 @@
         <v>91</v>
       </c>
       <c r="D43" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E43" s="65" t="s">
         <v>101</v>
       </c>
       <c r="F43" s="66"/>
       <c r="G43" s="48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H43" s="14">
         <v>40</v>
@@ -4374,7 +4381,7 @@
         <v>124</v>
       </c>
       <c r="J43" s="39" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="K43" s="59" t="s">
         <v>69</v>
@@ -4387,7 +4394,7 @@
         <v>62</v>
       </c>
       <c r="O43" s="46" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="P43" s="16" t="s">
         <v>19</v>
@@ -4402,10 +4409,10 @@
         <v>126</v>
       </c>
       <c r="T43" s="13" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="U43" s="61" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -4419,14 +4426,14 @@
         <v>91</v>
       </c>
       <c r="D44" s="62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E44" s="67" t="s">
         <v>101</v>
       </c>
       <c r="F44" s="63"/>
       <c r="G44" s="45" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="H44" s="9">
         <v>41</v>
@@ -4435,7 +4442,7 @@
         <v>124</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="K44" s="53" t="s">
         <v>69</v>
@@ -4446,7 +4453,7 @@
         <v>73</v>
       </c>
       <c r="O44" s="46" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P44" s="11" t="s">
         <v>20</v>
@@ -4461,7 +4468,7 @@
         <v>126</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="U44" s="55" t="s">
         <v>128</v>
@@ -4516,7 +4523,7 @@
       </c>
       <c r="F46" s="63"/>
       <c r="G46" s="45" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H46" s="9">
         <v>42</v>
@@ -4525,7 +4532,7 @@
         <v>124</v>
       </c>
       <c r="J46" s="27" t="s">
-        <v>241</v>
+        <v>317</v>
       </c>
       <c r="K46" s="53" t="s">
         <v>69</v>
@@ -4538,7 +4545,7 @@
         <v>50</v>
       </c>
       <c r="O46" s="46" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P46" s="11" t="s">
         <v>19</v>
@@ -4553,7 +4560,7 @@
         <v>126</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U46" s="55" t="s">
         <v>128</v>
@@ -4577,7 +4584,7 @@
       </c>
       <c r="F47" s="63"/>
       <c r="G47" s="45" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="H47" s="9">
         <v>43</v>
@@ -4586,7 +4593,7 @@
         <v>139</v>
       </c>
       <c r="J47" s="27" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="K47" s="53" t="s">
         <v>69</v>
@@ -4599,7 +4606,7 @@
       </c>
       <c r="N47" s="29"/>
       <c r="O47" s="46" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="P47" s="11" t="s">
         <v>19</v>
@@ -4614,7 +4621,7 @@
         <v>132</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="U47" s="55" t="s">
         <v>134</v>
@@ -4638,7 +4645,7 @@
       </c>
       <c r="F48" s="66"/>
       <c r="G48" s="48" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H48" s="9">
         <v>44</v>
@@ -4647,7 +4654,7 @@
         <v>124</v>
       </c>
       <c r="J48" s="39" t="s">
-        <v>242</v>
+        <v>318</v>
       </c>
       <c r="K48" s="59" t="s">
         <v>69</v>
@@ -4660,7 +4667,7 @@
         <v>62</v>
       </c>
       <c r="O48" s="49" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="P48" s="16" t="s">
         <v>19</v>
@@ -4675,10 +4682,10 @@
         <v>126</v>
       </c>
       <c r="T48" s="13" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="U48" s="61" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
@@ -4697,7 +4704,7 @@
       <c r="E49" s="67"/>
       <c r="F49" s="63"/>
       <c r="G49" s="45" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H49" s="9">
         <v>45</v>
@@ -4706,7 +4713,7 @@
         <v>124</v>
       </c>
       <c r="J49" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K49" s="53" t="s">
         <v>70</v>
@@ -4730,7 +4737,7 @@
         <v>151</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U49" s="55" t="s">
         <v>153</v>
@@ -4752,7 +4759,7 @@
       <c r="E50" s="67"/>
       <c r="F50" s="63"/>
       <c r="G50" s="45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H50" s="9">
         <v>46</v>
@@ -4761,7 +4768,7 @@
         <v>124</v>
       </c>
       <c r="J50" s="27" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="K50" s="53" t="s">
         <v>70</v>
@@ -4809,7 +4816,7 @@
       <c r="E51" s="67"/>
       <c r="F51" s="63"/>
       <c r="G51" s="45" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H51" s="9">
         <v>47</v>
@@ -4818,7 +4825,7 @@
         <v>124</v>
       </c>
       <c r="J51" s="27" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="K51" s="53" t="s">
         <v>69</v>
@@ -4831,7 +4838,7 @@
         <v>64</v>
       </c>
       <c r="O51" s="46" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="P51" s="11" t="s">
         <v>19</v>
@@ -4846,7 +4853,7 @@
         <v>126</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U51" s="55" t="s">
         <v>128</v>
@@ -4868,7 +4875,7 @@
       <c r="E52" s="67"/>
       <c r="F52" s="63"/>
       <c r="G52" s="48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H52" s="9">
         <v>48</v>
@@ -4877,7 +4884,7 @@
         <v>124</v>
       </c>
       <c r="J52" s="39" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="K52" s="59" t="s">
         <v>69</v>
@@ -4890,7 +4897,7 @@
         <v>62</v>
       </c>
       <c r="O52" s="49" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="P52" s="16" t="s">
         <v>19</v>
@@ -4905,10 +4912,10 @@
         <v>126</v>
       </c>
       <c r="T52" s="44" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="U52" s="44" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
@@ -4927,7 +4934,7 @@
       <c r="E53" s="67"/>
       <c r="F53" s="63"/>
       <c r="G53" s="45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H53" s="9">
         <v>49</v>
@@ -4936,7 +4943,7 @@
         <v>124</v>
       </c>
       <c r="J53" s="27" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="K53" s="53" t="s">
         <v>69</v>
@@ -4979,7 +4986,7 @@
         <v>124</v>
       </c>
       <c r="J54" s="27" t="s">
-        <v>257</v>
+        <v>319</v>
       </c>
       <c r="K54" s="53" t="s">
         <v>69</v>
@@ -4992,7 +4999,7 @@
         <v>23</v>
       </c>
       <c r="O54" s="46" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="P54" s="11" t="s">
         <v>19</v>
@@ -5007,7 +5014,7 @@
         <v>126</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="U54" s="55" t="s">
         <v>128</v>
@@ -5024,12 +5031,12 @@
         <v>91</v>
       </c>
       <c r="D55" s="64" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="E55" s="67"/>
       <c r="F55" s="63"/>
       <c r="G55" s="48" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="H55" s="9">
         <v>51</v>
@@ -5038,7 +5045,7 @@
         <v>124</v>
       </c>
       <c r="J55" s="39" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="K55" s="59" t="s">
         <v>69</v>
@@ -5051,7 +5058,7 @@
         <v>63</v>
       </c>
       <c r="O55" s="49" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="P55" s="11"/>
       <c r="Q55" s="50">

</xml_diff>